<commit_message>
Adding in demo for two length pCa
</commit_message>
<xml_diff>
--- a/code/demos/fitting/two_length_tension_pCa/target_data/target_force_pCa_data.xlsx
+++ b/code/demos/fitting/two_length_tension_pCa/target_data/target_force_pCa_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ken\GitHub\CampbellMuscleLab\models\MATMyoSim\code\demos\fitting\two_length_tension_pCa\target_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E24AA3-AE94-4BFF-9D9B-E355FC156E8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F59F9E7B-66E1-453E-9203-70F1AFDD9A35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="1650" windowWidth="24225" windowHeight="13950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="8">
   <si>
     <t>treatment</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>force</t>
-  </si>
-  <si>
-    <t>force_error</t>
   </si>
   <si>
     <t>curve</t>
@@ -406,7 +403,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -420,7 +417,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -434,9 +431,7 @@
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
@@ -454,9 +449,6 @@
       <c r="E2">
         <v>436.66666666666669</v>
       </c>
-      <c r="F2">
-        <v>91.802929026136084</v>
-      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
@@ -474,9 +466,6 @@
       <c r="E3">
         <v>661.11111111111109</v>
       </c>
-      <c r="F3">
-        <v>139.12868188643486</v>
-      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
@@ -494,9 +483,6 @@
       <c r="E4">
         <v>2231.1111111111113</v>
       </c>
-      <c r="F4">
-        <v>433.73841465297841</v>
-      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
@@ -514,9 +500,6 @@
       <c r="E5">
         <v>5122.2222222222226</v>
       </c>
-      <c r="F5">
-        <v>818.33295617400972</v>
-      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
@@ -534,9 +517,6 @@
       <c r="E6">
         <v>13652.222222222223</v>
       </c>
-      <c r="F6">
-        <v>950.45716745179732</v>
-      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
@@ -553,9 +533,6 @@
       </c>
       <c r="E7">
         <v>19701.111111111109</v>
-      </c>
-      <c r="F7">
-        <v>1221.3942902869978</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -574,9 +551,6 @@
       <c r="E8">
         <v>2063.3333333333335</v>
       </c>
-      <c r="F8">
-        <v>229.53455319648745</v>
-      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
@@ -594,9 +568,6 @@
       <c r="E9">
         <v>3536.6666666666665</v>
       </c>
-      <c r="F9">
-        <v>487.55911322514407</v>
-      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
@@ -614,9 +585,6 @@
       <c r="E10">
         <v>9827.7777777777774</v>
       </c>
-      <c r="F10">
-        <v>1415.0635809996684</v>
-      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
@@ -634,9 +602,6 @@
       <c r="E11">
         <v>14632.222222222223</v>
       </c>
-      <c r="F11">
-        <v>1841.5035959310969</v>
-      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
@@ -654,9 +619,6 @@
       <c r="E12">
         <v>22434.444444444445</v>
       </c>
-      <c r="F12">
-        <v>1635.5343257982076</v>
-      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
@@ -673,9 +635,6 @@
       </c>
       <c r="E13">
         <v>24100</v>
-      </c>
-      <c r="F13">
-        <v>1380.1871853725736</v>
       </c>
     </row>
   </sheetData>

</xml_diff>